<commit_message>
updated excel analysis for outliers, added images
</commit_message>
<xml_diff>
--- a/june_vs_december_analysis.xlsx
+++ b/june_vs_december_analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\twin_\Desktop\UofT CES - Data Analytics Boot Camp\Class Work\module 09\module_9_challenge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F8777A5-8B3D-4814-87C5-BF9FAC116DAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57A4DE9C-2328-41CF-9B23-6250F474910D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14020" yWindow="-16310" windowWidth="29020" windowHeight="15820" xr2:uid="{CC636051-5BCA-4402-8FB5-D2C789075B07}"/>
+    <workbookView xWindow="-11180" yWindow="-15860" windowWidth="25420" windowHeight="15370" xr2:uid="{CC636051-5BCA-4402-8FB5-D2C789075B07}"/>
   </bookViews>
   <sheets>
     <sheet name="raw - from module_9_challenge" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="58">
   <si>
     <t>prcp</t>
   </si>
@@ -204,13 +204,28 @@
   <si>
     <t>JUNE vs DECEMBER - Temperature Analysis by STATION</t>
   </si>
+  <si>
+    <t>IQR</t>
+  </si>
+  <si>
+    <t>Dec</t>
+  </si>
+  <si>
+    <t>precip</t>
+  </si>
+  <si>
+    <t>outlier</t>
+  </si>
+  <si>
+    <t>temp</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -569,32 +584,107 @@
     <xf numFmtId="9" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="7" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="5" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="5" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -604,88 +694,13 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="7" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="10" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="10" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="11" fillId="5" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="11" fillId="5" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="4">
     <dxf>
       <font>
         <color theme="0"/>
@@ -723,36 +738,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1066,10 +1051,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24D0AA94-7346-4B7D-B261-25FF3C75FD18}">
-  <dimension ref="A1:V90"/>
+  <sheetPr>
+    <pageSetUpPr autoPageBreaks="0"/>
+  </sheetPr>
+  <dimension ref="A1:AC90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O64" workbookViewId="0">
-      <selection activeCell="U87" sqref="U87"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="O58" workbookViewId="0">
+      <selection activeCell="P73" sqref="P73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" outlineLevelCol="1" x14ac:dyDescent="0.35"/>
@@ -1091,38 +1079,38 @@
     <col min="23" max="16384" width="8.7265625" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:22" ht="11.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:22" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="P2" s="28" t="s">
+    <row r="1" spans="2:29" ht="11.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:29" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="P2" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="Q2" s="29"/>
-      <c r="R2" s="29"/>
-      <c r="S2" s="29"/>
-      <c r="T2" s="29"/>
-      <c r="U2" s="29"/>
-      <c r="V2" s="30"/>
-    </row>
-    <row r="3" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="Q2" s="54"/>
+      <c r="R2" s="54"/>
+      <c r="S2" s="54"/>
+      <c r="T2" s="54"/>
+      <c r="U2" s="54"/>
+      <c r="V2" s="55"/>
+    </row>
+    <row r="3" spans="2:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="16" t="s">
         <v>9</v>
       </c>
       <c r="I3" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="P3" s="25"/>
-      <c r="Q3" s="19" t="s">
+      <c r="P3" s="23"/>
+      <c r="Q3" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="R3" s="20"/>
-      <c r="S3" s="26"/>
-      <c r="T3" s="19" t="s">
+      <c r="R3" s="46"/>
+      <c r="S3" s="24"/>
+      <c r="T3" s="45" t="s">
         <v>38</v>
       </c>
-      <c r="U3" s="20"/>
-      <c r="V3" s="27"/>
-    </row>
-    <row r="4" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="U3" s="46"/>
+      <c r="V3" s="25"/>
+    </row>
+    <row r="4" spans="2:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="17"/>
       <c r="C4" s="2" t="s">
         <v>0</v>
@@ -1151,13 +1139,13 @@
         <v>3</v>
       </c>
       <c r="P4" s="1"/>
-      <c r="Q4" s="49" t="s">
+      <c r="Q4" s="39" t="s">
         <v>35</v>
       </c>
       <c r="R4" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="S4" s="24" t="s">
+      <c r="S4" s="22" t="s">
         <v>36</v>
       </c>
       <c r="T4" s="1" t="s">
@@ -1166,11 +1154,11 @@
       <c r="U4" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="V4" s="24" t="s">
+      <c r="V4" s="22" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:29" x14ac:dyDescent="0.35">
       <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
@@ -1212,7 +1200,7 @@
         <f>J5</f>
         <v>1405</v>
       </c>
-      <c r="S5" s="21" t="str">
+      <c r="S5" s="19" t="str">
         <f>IF(Q5&gt;R5,Q$4,R$4)&amp;" by "&amp;IF(Q5&gt;R5,Q5-R5,R5-Q5)</f>
         <v>June by 169</v>
       </c>
@@ -1224,12 +1212,12 @@
         <f>K5</f>
         <v>1517</v>
       </c>
-      <c r="V5" s="21" t="str">
+      <c r="V5" s="19" t="str">
         <f>IF(T5&gt;U5,T$4,U$4)&amp;" by "&amp;IF(T5&gt;U5,T5-U5,U5-T5)</f>
         <v>June by 183</v>
       </c>
     </row>
-    <row r="6" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:29" x14ac:dyDescent="0.35">
       <c r="B6" s="4" t="s">
         <v>5</v>
       </c>
@@ -1271,7 +1259,7 @@
         <f t="shared" ref="R6:R12" si="1">J6</f>
         <v>0.21681900000000001</v>
       </c>
-      <c r="S6" s="22" t="str">
+      <c r="S6" s="20" t="str">
         <f t="shared" ref="S6:S12" si="2">IF(Q6&gt;R6,Q$4,R$4)&amp;" by "&amp;IF(Q6&gt;R6,Q6-R6,R6-Q6)</f>
         <v>December by 0.080459</v>
       </c>
@@ -1283,12 +1271,12 @@
         <f t="shared" ref="U6:U12" si="4">K6</f>
         <v>71.041528999999997</v>
       </c>
-      <c r="V6" s="22" t="str">
+      <c r="V6" s="20" t="str">
         <f t="shared" ref="V6:V12" si="5">IF(T6&gt;U6,T$4,U$4)&amp;" by "&amp;IF(T6&gt;U6,T6-U6,U6-T6)</f>
         <v>June by 3.90258900000001</v>
       </c>
     </row>
-    <row r="7" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:29" x14ac:dyDescent="0.35">
       <c r="B7" s="4" t="s">
         <v>6</v>
       </c>
@@ -1330,7 +1318,7 @@
         <f t="shared" si="1"/>
         <v>0.54139899999999996</v>
       </c>
-      <c r="S7" s="22" t="str">
+      <c r="S7" s="20" t="str">
         <f t="shared" si="2"/>
         <v>December by 0.205668</v>
       </c>
@@ -1342,12 +1330,18 @@
         <f t="shared" si="4"/>
         <v>3.7459199999999999</v>
       </c>
-      <c r="V7" s="22" t="str">
+      <c r="V7" s="20" t="str">
         <f t="shared" si="5"/>
         <v>December by 0.488503</v>
       </c>
-    </row>
-    <row r="8" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="Y7" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB7" s="15" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="2:29" x14ac:dyDescent="0.35">
       <c r="B8" s="4" t="s">
         <v>7</v>
       </c>
@@ -1389,7 +1383,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S8" s="22" t="str">
+      <c r="S8" s="20" t="str">
         <f t="shared" si="2"/>
         <v>December by 0</v>
       </c>
@@ -1401,12 +1395,24 @@
         <f t="shared" si="4"/>
         <v>56</v>
       </c>
-      <c r="V8" s="22" t="str">
+      <c r="V8" s="20" t="str">
         <f t="shared" si="5"/>
         <v>June by 8</v>
       </c>
-    </row>
-    <row r="9" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="Y8" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z8" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB8" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC8" s="15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="2:29" x14ac:dyDescent="0.35">
       <c r="B9" s="18">
         <v>0.25</v>
       </c>
@@ -1448,7 +1454,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S9" s="22" t="str">
+      <c r="S9" s="20" t="str">
         <f t="shared" si="2"/>
         <v>December by 0</v>
       </c>
@@ -1460,12 +1466,31 @@
         <f t="shared" si="4"/>
         <v>69</v>
       </c>
-      <c r="V9" s="22" t="str">
+      <c r="V9" s="20" t="str">
         <f t="shared" si="5"/>
         <v>June by 4</v>
       </c>
-    </row>
-    <row r="10" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="X9" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y9" s="15">
+        <f>Q11-Q9</f>
+        <v>0.12</v>
+      </c>
+      <c r="Z9" s="15">
+        <f>R11-R9</f>
+        <v>0.15</v>
+      </c>
+      <c r="AB9" s="15">
+        <f>T11-T9</f>
+        <v>4</v>
+      </c>
+      <c r="AC9" s="15">
+        <f>U11-U9</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="2:29" x14ac:dyDescent="0.35">
       <c r="B10" s="18">
         <v>0.5</v>
       </c>
@@ -1507,7 +1532,7 @@
         <f t="shared" si="1"/>
         <v>0.03</v>
       </c>
-      <c r="S10" s="22" t="str">
+      <c r="S10" s="20" t="str">
         <f t="shared" si="2"/>
         <v>December by 0.01</v>
       </c>
@@ -1519,12 +1544,31 @@
         <f t="shared" si="4"/>
         <v>71</v>
       </c>
-      <c r="V10" s="22" t="str">
+      <c r="V10" s="20" t="str">
         <f t="shared" si="5"/>
         <v>June by 4</v>
       </c>
-    </row>
-    <row r="11" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="X10" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y10" s="15">
+        <f>Q11+(1.5*Y9)</f>
+        <v>0.3</v>
+      </c>
+      <c r="Z10" s="15">
+        <f>R11+(1.5*Z9)</f>
+        <v>0.375</v>
+      </c>
+      <c r="AB10" s="15">
+        <f>T11+(1.5*AB9)</f>
+        <v>83</v>
+      </c>
+      <c r="AC10" s="15">
+        <f>U11+(1.5*AC9)</f>
+        <v>81.5</v>
+      </c>
+    </row>
+    <row r="11" spans="2:29" x14ac:dyDescent="0.35">
       <c r="B11" s="18">
         <v>0.75</v>
       </c>
@@ -1566,7 +1610,7 @@
         <f t="shared" si="1"/>
         <v>0.15</v>
       </c>
-      <c r="S11" s="22" t="str">
+      <c r="S11" s="20" t="str">
         <f t="shared" si="2"/>
         <v>December by 0.03</v>
       </c>
@@ -1578,12 +1622,12 @@
         <f t="shared" si="4"/>
         <v>74</v>
       </c>
-      <c r="V11" s="22" t="str">
+      <c r="V11" s="20" t="str">
         <f t="shared" si="5"/>
         <v>June by 3</v>
       </c>
     </row>
-    <row r="12" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B12" s="7" t="s">
         <v>8</v>
       </c>
@@ -1625,7 +1669,7 @@
         <f t="shared" si="1"/>
         <v>6.42</v>
       </c>
-      <c r="S12" s="23" t="str">
+      <c r="S12" s="21" t="str">
         <f t="shared" si="2"/>
         <v>December by 1.99</v>
       </c>
@@ -1637,41 +1681,41 @@
         <f t="shared" si="4"/>
         <v>83</v>
       </c>
-      <c r="V12" s="23" t="str">
+      <c r="V12" s="21" t="str">
         <f t="shared" si="5"/>
         <v>June by 2</v>
       </c>
     </row>
-    <row r="13" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="14" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="P14" s="31" t="s">
+    <row r="13" spans="2:29" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="14" spans="2:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="P14" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="Q14" s="32"/>
-      <c r="R14" s="32"/>
-      <c r="S14" s="32"/>
-      <c r="T14" s="32"/>
-      <c r="U14" s="33"/>
-    </row>
-    <row r="15" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="Q14" s="48"/>
+      <c r="R14" s="48"/>
+      <c r="S14" s="48"/>
+      <c r="T14" s="48"/>
+      <c r="U14" s="49"/>
+    </row>
+    <row r="15" spans="2:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B15" s="16" t="s">
         <v>11</v>
       </c>
       <c r="I15" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="P15" s="25"/>
-      <c r="Q15" s="19" t="s">
+      <c r="P15" s="23"/>
+      <c r="Q15" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="R15" s="20"/>
-      <c r="S15" s="26"/>
-      <c r="T15" s="19" t="s">
+      <c r="R15" s="46"/>
+      <c r="S15" s="24"/>
+      <c r="T15" s="45" t="s">
         <v>43</v>
       </c>
-      <c r="U15" s="20"/>
-    </row>
-    <row r="16" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="U15" s="46"/>
+    </row>
+    <row r="16" spans="2:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B16" s="1" t="s">
         <v>3</v>
       </c>
@@ -1711,13 +1755,13 @@
       <c r="P16" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="Q16" s="49" t="s">
+      <c r="Q16" s="39" t="s">
         <v>35</v>
       </c>
       <c r="R16" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="S16" s="24" t="s">
+      <c r="S16" s="22" t="s">
         <v>36</v>
       </c>
       <c r="T16" s="1" t="s">
@@ -1775,12 +1819,12 @@
         <f>L17</f>
         <v>230</v>
       </c>
-      <c r="S17" s="21" t="str">
-        <f>IF(Q17&gt;R17,Q$16,R$16)&amp;" by "&amp;IF(Q17&gt;R17,Q17-R17,R17-Q17)</f>
+      <c r="S17" s="19" t="str">
+        <f t="shared" ref="S17:S24" si="6">IF(Q17&gt;R17,Q$16,R$16)&amp;" by "&amp;IF(Q17&gt;R17,Q17-R17,R17-Q17)</f>
         <v>June by 2</v>
       </c>
-      <c r="T17" s="35"/>
-      <c r="U17" s="36"/>
+      <c r="T17" s="27"/>
+      <c r="U17" s="28"/>
     </row>
     <row r="18" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B18" s="4">
@@ -1823,22 +1867,22 @@
         <v>2011</v>
       </c>
       <c r="Q18" s="6">
-        <f t="shared" ref="Q18:Q24" si="6">E18</f>
+        <f t="shared" ref="Q18:Q24" si="7">E18</f>
         <v>212</v>
       </c>
       <c r="R18" s="12">
-        <f t="shared" ref="R18:R23" si="7">L18</f>
+        <f t="shared" ref="R18:R23" si="8">L18</f>
         <v>215</v>
       </c>
-      <c r="S18" s="22" t="str">
-        <f>IF(Q18&gt;R18,Q$16,R$16)&amp;" by "&amp;IF(Q18&gt;R18,Q18-R18,R18-Q18)</f>
+      <c r="S18" s="20" t="str">
+        <f t="shared" si="6"/>
         <v>December by 3</v>
       </c>
-      <c r="T18" s="39">
+      <c r="T18" s="29">
         <f>(Q18-Q17)/Q17</f>
         <v>-8.6206896551724144E-2</v>
       </c>
-      <c r="U18" s="40">
+      <c r="U18" s="30">
         <f>(R18-R17)/R17</f>
         <v>-6.5217391304347824E-2</v>
       </c>
@@ -1884,23 +1928,23 @@
         <v>2012</v>
       </c>
       <c r="Q19" s="6">
+        <f t="shared" si="7"/>
+        <v>194</v>
+      </c>
+      <c r="R19" s="12">
+        <f t="shared" si="8"/>
+        <v>202</v>
+      </c>
+      <c r="S19" s="20" t="str">
         <f t="shared" si="6"/>
-        <v>194</v>
-      </c>
-      <c r="R19" s="12">
-        <f t="shared" si="7"/>
-        <v>202</v>
-      </c>
-      <c r="S19" s="22" t="str">
-        <f>IF(Q19&gt;R19,Q$16,R$16)&amp;" by "&amp;IF(Q19&gt;R19,Q19-R19,R19-Q19)</f>
         <v>December by 8</v>
       </c>
-      <c r="T19" s="41">
-        <f t="shared" ref="T19:T24" si="8">(Q19-Q18)/Q18</f>
+      <c r="T19" s="31">
+        <f t="shared" ref="T19:T24" si="9">(Q19-Q18)/Q18</f>
         <v>-8.4905660377358486E-2</v>
       </c>
-      <c r="U19" s="42">
-        <f t="shared" ref="U19:U24" si="9">(R19-R18)/R18</f>
+      <c r="U19" s="32">
+        <f t="shared" ref="U19:U24" si="10">(R19-R18)/R18</f>
         <v>-6.0465116279069767E-2</v>
       </c>
     </row>
@@ -1945,23 +1989,23 @@
         <v>2013</v>
       </c>
       <c r="Q20" s="6">
+        <f t="shared" si="7"/>
+        <v>205</v>
+      </c>
+      <c r="R20" s="12">
+        <f t="shared" si="8"/>
+        <v>213</v>
+      </c>
+      <c r="S20" s="20" t="str">
         <f t="shared" si="6"/>
-        <v>205</v>
-      </c>
-      <c r="R20" s="12">
-        <f t="shared" si="7"/>
-        <v>213</v>
-      </c>
-      <c r="S20" s="22" t="str">
-        <f>IF(Q20&gt;R20,Q$16,R$16)&amp;" by "&amp;IF(Q20&gt;R20,Q20-R20,R20-Q20)</f>
         <v>December by 8</v>
       </c>
-      <c r="T20" s="41">
-        <f t="shared" si="8"/>
+      <c r="T20" s="31">
+        <f t="shared" si="9"/>
         <v>5.6701030927835051E-2</v>
       </c>
-      <c r="U20" s="42">
-        <f t="shared" si="9"/>
+      <c r="U20" s="32">
+        <f t="shared" si="10"/>
         <v>5.4455445544554455E-2</v>
       </c>
     </row>
@@ -2006,23 +2050,23 @@
         <v>2014</v>
       </c>
       <c r="Q21" s="6">
+        <f t="shared" si="7"/>
+        <v>199</v>
+      </c>
+      <c r="R21" s="12">
+        <f t="shared" si="8"/>
+        <v>205</v>
+      </c>
+      <c r="S21" s="20" t="str">
         <f t="shared" si="6"/>
-        <v>199</v>
-      </c>
-      <c r="R21" s="12">
-        <f t="shared" si="7"/>
-        <v>205</v>
-      </c>
-      <c r="S21" s="22" t="str">
-        <f>IF(Q21&gt;R21,Q$16,R$16)&amp;" by "&amp;IF(Q21&gt;R21,Q21-R21,R21-Q21)</f>
         <v>December by 6</v>
       </c>
-      <c r="T21" s="41">
-        <f t="shared" si="8"/>
+      <c r="T21" s="31">
+        <f t="shared" si="9"/>
         <v>-2.9268292682926831E-2</v>
       </c>
-      <c r="U21" s="42">
-        <f t="shared" si="9"/>
+      <c r="U21" s="32">
+        <f t="shared" si="10"/>
         <v>-3.7558685446009391E-2</v>
       </c>
     </row>
@@ -2067,23 +2111,23 @@
         <v>2015</v>
       </c>
       <c r="Q22" s="6">
+        <f t="shared" si="7"/>
+        <v>188</v>
+      </c>
+      <c r="R22" s="12">
+        <f t="shared" si="8"/>
+        <v>162</v>
+      </c>
+      <c r="S22" s="20" t="str">
         <f t="shared" si="6"/>
-        <v>188</v>
-      </c>
-      <c r="R22" s="12">
-        <f t="shared" si="7"/>
-        <v>162</v>
-      </c>
-      <c r="S22" s="22" t="str">
-        <f>IF(Q22&gt;R22,Q$16,R$16)&amp;" by "&amp;IF(Q22&gt;R22,Q22-R22,R22-Q22)</f>
         <v>June by 26</v>
       </c>
-      <c r="T22" s="41">
-        <f t="shared" si="8"/>
+      <c r="T22" s="31">
+        <f t="shared" si="9"/>
         <v>-5.5276381909547742E-2</v>
       </c>
-      <c r="U22" s="42">
-        <f t="shared" si="9"/>
+      <c r="U22" s="32">
+        <f t="shared" si="10"/>
         <v>-0.2097560975609756</v>
       </c>
     </row>
@@ -2128,23 +2172,23 @@
         <v>2016</v>
       </c>
       <c r="Q23" s="6">
+        <f t="shared" si="7"/>
+        <v>173</v>
+      </c>
+      <c r="R23" s="12">
+        <f t="shared" si="8"/>
+        <v>178</v>
+      </c>
+      <c r="S23" s="20" t="str">
         <f t="shared" si="6"/>
-        <v>173</v>
-      </c>
-      <c r="R23" s="12">
-        <f t="shared" si="7"/>
-        <v>178</v>
-      </c>
-      <c r="S23" s="22" t="str">
-        <f>IF(Q23&gt;R23,Q$16,R$16)&amp;" by "&amp;IF(Q23&gt;R23,Q23-R23,R23-Q23)</f>
         <v>December by 5</v>
       </c>
-      <c r="T23" s="41">
-        <f t="shared" si="8"/>
+      <c r="T23" s="31">
+        <f t="shared" si="9"/>
         <v>-7.9787234042553196E-2</v>
       </c>
-      <c r="U23" s="42">
-        <f t="shared" si="9"/>
+      <c r="U23" s="32">
+        <f t="shared" si="10"/>
         <v>9.8765432098765427E-2</v>
       </c>
     </row>
@@ -2171,55 +2215,55 @@
         <v>41</v>
       </c>
       <c r="Q24" s="8">
+        <f t="shared" si="7"/>
+        <v>171</v>
+      </c>
+      <c r="R24" s="38"/>
+      <c r="S24" s="21" t="str">
         <f t="shared" si="6"/>
-        <v>171</v>
-      </c>
-      <c r="R24" s="48"/>
-      <c r="S24" s="23" t="str">
-        <f>IF(Q24&gt;R24,Q$16,R$16)&amp;" by "&amp;IF(Q24&gt;R24,Q24-R24,R24-Q24)</f>
         <v>June by 171</v>
       </c>
-      <c r="T24" s="43">
-        <f t="shared" si="8"/>
+      <c r="T24" s="33">
+        <f t="shared" si="9"/>
         <v>-1.1560693641618497E-2</v>
       </c>
-      <c r="U24" s="44">
-        <f t="shared" si="9"/>
+      <c r="U24" s="34">
+        <f t="shared" si="10"/>
         <v>-1</v>
       </c>
     </row>
     <row r="25" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="P25" s="37" t="s">
+      <c r="P25" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="Q25" s="37"/>
-      <c r="R25" s="37"/>
-      <c r="S25" s="45" t="s">
+      <c r="Q25" s="50"/>
+      <c r="R25" s="50"/>
+      <c r="S25" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="T25" s="46">
+      <c r="T25" s="36">
         <f>(Q23-Q17)/Q17</f>
         <v>-0.25431034482758619</v>
       </c>
-      <c r="U25" s="47">
+      <c r="U25" s="37">
         <f>(R23-R17)/R17</f>
         <v>-0.22608695652173913</v>
       </c>
     </row>
     <row r="26" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="P26" s="38"/>
-      <c r="Q26" s="38"/>
-      <c r="R26" s="38"/>
+      <c r="P26" s="52"/>
+      <c r="Q26" s="52"/>
+      <c r="R26" s="52"/>
     </row>
     <row r="27" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="P27" s="31" t="s">
+      <c r="P27" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="Q27" s="32"/>
-      <c r="R27" s="32"/>
-      <c r="S27" s="32"/>
-      <c r="T27" s="32"/>
-      <c r="U27" s="33"/>
+      <c r="Q27" s="48"/>
+      <c r="R27" s="48"/>
+      <c r="S27" s="48"/>
+      <c r="T27" s="48"/>
+      <c r="U27" s="49"/>
     </row>
     <row r="28" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B28" s="16" t="s">
@@ -2228,16 +2272,16 @@
       <c r="I28" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="P28" s="25"/>
-      <c r="Q28" s="19" t="s">
+      <c r="P28" s="23"/>
+      <c r="Q28" s="45" t="s">
         <v>45</v>
       </c>
-      <c r="R28" s="20"/>
-      <c r="S28" s="26"/>
-      <c r="T28" s="19" t="s">
+      <c r="R28" s="46"/>
+      <c r="S28" s="24"/>
+      <c r="T28" s="45" t="s">
         <v>43</v>
       </c>
-      <c r="U28" s="20"/>
+      <c r="U28" s="46"/>
     </row>
     <row r="29" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B29" s="1" t="s">
@@ -2267,13 +2311,13 @@
       <c r="P29" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="Q29" s="49" t="s">
+      <c r="Q29" s="39" t="s">
         <v>35</v>
       </c>
       <c r="R29" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="S29" s="24" t="s">
+      <c r="S29" s="22" t="s">
         <v>36</v>
       </c>
       <c r="T29" s="1" t="s">
@@ -2319,12 +2363,12 @@
         <f>J30</f>
         <v>105.59</v>
       </c>
-      <c r="S30" s="21" t="str">
-        <f>IF(Q30&gt;R30,Q$16,R$16)&amp;" by "&amp;IF(Q30&gt;R30,Q30-R30,R30-Q30)</f>
+      <c r="S30" s="19" t="str">
+        <f t="shared" ref="S30:S37" si="11">IF(Q30&gt;R30,Q$16,R$16)&amp;" by "&amp;IF(Q30&gt;R30,Q30-R30,R30-Q30)</f>
         <v>December by 95.79</v>
       </c>
-      <c r="T30" s="35"/>
-      <c r="U30" s="36"/>
+      <c r="T30" s="27"/>
+      <c r="U30" s="28"/>
     </row>
     <row r="31" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B31" s="4">
@@ -2355,22 +2399,22 @@
         <v>2011</v>
       </c>
       <c r="Q31" s="6">
-        <f t="shared" ref="Q31:Q37" si="10">C31</f>
+        <f t="shared" ref="Q31:Q37" si="12">C31</f>
         <v>50.91</v>
       </c>
       <c r="R31" s="12">
-        <f t="shared" ref="R31:R36" si="11">J31</f>
+        <f t="shared" ref="R31:R36" si="13">J31</f>
         <v>43.34</v>
       </c>
-      <c r="S31" s="22" t="str">
-        <f>IF(Q31&gt;R31,Q$16,R$16)&amp;" by "&amp;IF(Q31&gt;R31,Q31-R31,R31-Q31)</f>
+      <c r="S31" s="20" t="str">
+        <f t="shared" si="11"/>
         <v>June by 7.56999999999999</v>
       </c>
-      <c r="T31" s="39">
+      <c r="T31" s="29">
         <f>(Q31-Q30)/Q30</f>
         <v>4.194897959183673</v>
       </c>
-      <c r="U31" s="40">
+      <c r="U31" s="30">
         <f>(R31-R30)/R30</f>
         <v>-0.58954446443792019</v>
       </c>
@@ -2404,23 +2448,23 @@
         <v>2012</v>
       </c>
       <c r="Q32" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>18.829999999999998</v>
       </c>
       <c r="R32" s="12">
+        <f t="shared" si="13"/>
+        <v>18.100000000000001</v>
+      </c>
+      <c r="S32" s="20" t="str">
         <f t="shared" si="11"/>
-        <v>18.100000000000001</v>
-      </c>
-      <c r="S32" s="22" t="str">
-        <f>IF(Q32&gt;R32,Q$16,R$16)&amp;" by "&amp;IF(Q32&gt;R32,Q32-R32,R32-Q32)</f>
         <v>June by 0.729999999999997</v>
       </c>
-      <c r="T32" s="41">
-        <f t="shared" ref="T32:T37" si="12">(Q32-Q31)/Q31</f>
+      <c r="T32" s="31">
+        <f t="shared" ref="T32:T37" si="14">(Q32-Q31)/Q31</f>
         <v>-0.63013160479277153</v>
       </c>
-      <c r="U32" s="42">
-        <f t="shared" ref="U32:U37" si="13">(R32-R31)/R31</f>
+      <c r="U32" s="32">
+        <f t="shared" ref="U32:U37" si="15">(R32-R31)/R31</f>
         <v>-0.58237194277803417</v>
       </c>
     </row>
@@ -2453,23 +2497,23 @@
         <v>2013</v>
       </c>
       <c r="Q33" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>29.56</v>
       </c>
       <c r="R33" s="12">
+        <f t="shared" si="13"/>
+        <v>36</v>
+      </c>
+      <c r="S33" s="20" t="str">
         <f t="shared" si="11"/>
-        <v>36</v>
-      </c>
-      <c r="S33" s="22" t="str">
-        <f>IF(Q33&gt;R33,Q$16,R$16)&amp;" by "&amp;IF(Q33&gt;R33,Q33-R33,R33-Q33)</f>
         <v>December by 6.44</v>
       </c>
-      <c r="T33" s="41">
-        <f t="shared" si="12"/>
+      <c r="T33" s="31">
+        <f t="shared" si="14"/>
         <v>0.56983536909187471</v>
       </c>
-      <c r="U33" s="42">
-        <f t="shared" si="13"/>
+      <c r="U33" s="32">
+        <f t="shared" si="15"/>
         <v>0.98895027624309373</v>
       </c>
     </row>
@@ -2502,23 +2546,23 @@
         <v>2014</v>
       </c>
       <c r="Q34" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>24.75</v>
       </c>
       <c r="R34" s="12">
+        <f t="shared" si="13"/>
+        <v>38.630000000000003</v>
+      </c>
+      <c r="S34" s="20" t="str">
         <f t="shared" si="11"/>
-        <v>38.630000000000003</v>
-      </c>
-      <c r="S34" s="22" t="str">
-        <f>IF(Q34&gt;R34,Q$16,R$16)&amp;" by "&amp;IF(Q34&gt;R34,Q34-R34,R34-Q34)</f>
         <v>December by 13.88</v>
       </c>
-      <c r="T34" s="41">
-        <f t="shared" si="12"/>
+      <c r="T34" s="31">
+        <f t="shared" si="14"/>
         <v>-0.16271989174560214</v>
       </c>
-      <c r="U34" s="42">
-        <f t="shared" si="13"/>
+      <c r="U34" s="32">
+        <f t="shared" si="15"/>
         <v>7.3055555555555624E-2</v>
       </c>
     </row>
@@ -2551,23 +2595,23 @@
         <v>2015</v>
       </c>
       <c r="Q35" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>23.53</v>
       </c>
       <c r="R35" s="12">
+        <f t="shared" si="13"/>
+        <v>27.46</v>
+      </c>
+      <c r="S35" s="20" t="str">
         <f t="shared" si="11"/>
-        <v>27.46</v>
-      </c>
-      <c r="S35" s="22" t="str">
-        <f>IF(Q35&gt;R35,Q$16,R$16)&amp;" by "&amp;IF(Q35&gt;R35,Q35-R35,R35-Q35)</f>
         <v>December by 3.93</v>
       </c>
-      <c r="T35" s="41">
-        <f t="shared" si="12"/>
+      <c r="T35" s="31">
+        <f t="shared" si="14"/>
         <v>-4.929292929292925E-2</v>
       </c>
-      <c r="U35" s="42">
-        <f t="shared" si="13"/>
+      <c r="U35" s="32">
+        <f t="shared" si="15"/>
         <v>-0.28915350763655195</v>
       </c>
     </row>
@@ -2600,23 +2644,23 @@
         <v>2016</v>
       </c>
       <c r="Q36" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>36.729999999999997</v>
       </c>
       <c r="R36" s="12">
+        <f t="shared" si="13"/>
+        <v>35.51</v>
+      </c>
+      <c r="S36" s="20" t="str">
         <f t="shared" si="11"/>
-        <v>35.51</v>
-      </c>
-      <c r="S36" s="22" t="str">
-        <f>IF(Q36&gt;R36,Q$16,R$16)&amp;" by "&amp;IF(Q36&gt;R36,Q36-R36,R36-Q36)</f>
         <v>June by 1.22</v>
       </c>
-      <c r="T36" s="41">
-        <f t="shared" si="12"/>
+      <c r="T36" s="31">
+        <f t="shared" si="14"/>
         <v>0.56098597535061601</v>
       </c>
-      <c r="U36" s="42">
-        <f t="shared" si="13"/>
+      <c r="U36" s="32">
+        <f t="shared" si="15"/>
         <v>0.29315367807720311</v>
       </c>
     </row>
@@ -2637,69 +2681,69 @@
         <v>41</v>
       </c>
       <c r="Q37" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>20.52</v>
       </c>
-      <c r="R37" s="48"/>
-      <c r="S37" s="23" t="str">
-        <f>IF(Q37&gt;R37,Q$16,R$16)&amp;" by "&amp;IF(Q37&gt;R37,Q37-R37,R37-Q37)</f>
+      <c r="R37" s="38"/>
+      <c r="S37" s="21" t="str">
+        <f t="shared" si="11"/>
         <v>June by 20.52</v>
       </c>
-      <c r="T37" s="43">
-        <f t="shared" si="12"/>
+      <c r="T37" s="33">
+        <f t="shared" si="14"/>
         <v>-0.44132861421181591</v>
       </c>
-      <c r="U37" s="44">
-        <f t="shared" si="13"/>
+      <c r="U37" s="34">
+        <f t="shared" si="15"/>
         <v>-1</v>
       </c>
     </row>
     <row r="38" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="P38" s="37" t="s">
+      <c r="P38" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="Q38" s="37"/>
-      <c r="R38" s="37"/>
-      <c r="S38" s="45" t="s">
+      <c r="Q38" s="50"/>
+      <c r="R38" s="50"/>
+      <c r="S38" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="T38" s="46">
+      <c r="T38" s="36">
         <f>(Q36-Q30)/Q30</f>
         <v>2.7479591836734687</v>
       </c>
-      <c r="U38" s="47">
+      <c r="U38" s="37">
         <f>(R36-R30)/R30</f>
         <v>-0.66369921394071418</v>
       </c>
     </row>
     <row r="39" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="P39" s="38"/>
-      <c r="Q39" s="38"/>
-      <c r="R39" s="38"/>
-      <c r="S39" s="45" t="s">
+      <c r="P39" s="52"/>
+      <c r="Q39" s="52"/>
+      <c r="R39" s="52"/>
+      <c r="S39" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="T39" s="46">
+      <c r="T39" s="36">
         <f>(Q36-Q31)/Q31</f>
         <v>-0.27853074052249066</v>
       </c>
-      <c r="U39" s="47">
+      <c r="U39" s="37">
         <f>(R36-R31)/R31</f>
         <v>-0.18066451315182291</v>
       </c>
-      <c r="V39" s="34" t="s">
+      <c r="V39" s="26" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="40" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="P40" s="31" t="s">
+      <c r="P40" s="47" t="s">
         <v>50</v>
       </c>
-      <c r="Q40" s="32"/>
-      <c r="R40" s="32"/>
-      <c r="S40" s="32"/>
-      <c r="T40" s="32"/>
-      <c r="U40" s="33"/>
+      <c r="Q40" s="48"/>
+      <c r="R40" s="48"/>
+      <c r="S40" s="48"/>
+      <c r="T40" s="48"/>
+      <c r="U40" s="49"/>
     </row>
     <row r="41" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B41" s="16" t="s">
@@ -2708,16 +2752,16 @@
       <c r="I41" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="P41" s="25"/>
-      <c r="Q41" s="19" t="s">
+      <c r="P41" s="23"/>
+      <c r="Q41" s="45" t="s">
         <v>48</v>
       </c>
-      <c r="R41" s="20"/>
-      <c r="S41" s="26"/>
-      <c r="T41" s="19" t="s">
+      <c r="R41" s="46"/>
+      <c r="S41" s="24"/>
+      <c r="T41" s="45" t="s">
         <v>43</v>
       </c>
-      <c r="U41" s="20"/>
+      <c r="U41" s="46"/>
     </row>
     <row r="42" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B42" s="1" t="s">
@@ -2753,7 +2797,7 @@
       <c r="R42" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="S42" s="24" t="s">
+      <c r="S42" s="22" t="s">
         <v>36</v>
       </c>
       <c r="T42" s="1" t="s">
@@ -2799,12 +2843,12 @@
         <f>K43</f>
         <v>70.208511000000001</v>
       </c>
-      <c r="S43" s="51" t="str">
-        <f>IF(Q43&gt;R43,Q$16,R$16)&amp;" by "&amp;IF(Q43&gt;R43,Q43-R43,R43-Q43)</f>
+      <c r="S43" s="41" t="str">
+        <f t="shared" ref="S43:S50" si="16">IF(Q43&gt;R43,Q$16,R$16)&amp;" by "&amp;IF(Q43&gt;R43,Q43-R43,R43-Q43)</f>
         <v>June by 4.71710899999999</v>
       </c>
-      <c r="T43" s="35"/>
-      <c r="U43" s="36"/>
+      <c r="T43" s="27"/>
+      <c r="U43" s="28"/>
     </row>
     <row r="44" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B44" s="4">
@@ -2835,22 +2879,22 @@
         <v>2011</v>
       </c>
       <c r="Q44" s="6">
-        <f t="shared" ref="Q44:Q50" si="14">D44</f>
+        <f t="shared" ref="Q44:Q50" si="17">D44</f>
         <v>73.938326000000004</v>
       </c>
       <c r="R44" s="12">
-        <f t="shared" ref="R44:R49" si="15">K44</f>
+        <f t="shared" ref="R44:R49" si="18">K44</f>
         <v>70.820627999999999</v>
       </c>
-      <c r="S44" s="52" t="str">
-        <f>IF(Q44&gt;R44,Q$16,R$16)&amp;" by "&amp;IF(Q44&gt;R44,Q44-R44,R44-Q44)</f>
+      <c r="S44" s="42" t="str">
+        <f t="shared" si="16"/>
         <v>June by 3.117698</v>
       </c>
-      <c r="T44" s="39">
+      <c r="T44" s="29">
         <f>(Q44-Q43)/Q43</f>
         <v>-1.3176988058290229E-2</v>
       </c>
-      <c r="U44" s="40">
+      <c r="U44" s="30">
         <f>(R44-R43)/R43</f>
         <v>8.7185583525620954E-3</v>
       </c>
@@ -2884,23 +2928,23 @@
         <v>2012</v>
       </c>
       <c r="Q45" s="6">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>74</v>
       </c>
       <c r="R45" s="12">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>71.188073000000003</v>
       </c>
-      <c r="S45" s="52" t="str">
-        <f>IF(Q45&gt;R45,Q$16,R$16)&amp;" by "&amp;IF(Q45&gt;R45,Q45-R45,R45-Q45)</f>
+      <c r="S45" s="42" t="str">
+        <f t="shared" si="16"/>
         <v>June by 2.811927</v>
       </c>
-      <c r="T45" s="41">
-        <f t="shared" ref="T45:T50" si="16">(Q45-Q44)/Q44</f>
+      <c r="T45" s="31">
+        <f t="shared" ref="T45:T50" si="19">(Q45-Q44)/Q44</f>
         <v>8.3412762144488431E-4</v>
       </c>
-      <c r="U45" s="42">
-        <f t="shared" ref="U45:U50" si="17">(R45-R44)/R44</f>
+      <c r="U45" s="32">
+        <f t="shared" ref="U45:U50" si="20">(R45-R44)/R44</f>
         <v>5.1883894618952485E-3</v>
       </c>
     </row>
@@ -2933,23 +2977,23 @@
         <v>2013</v>
       </c>
       <c r="Q46" s="6">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>74.599078000000006</v>
       </c>
       <c r="R46" s="12">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>71.094016999999994</v>
       </c>
-      <c r="S46" s="52" t="str">
-        <f>IF(Q46&gt;R46,Q$16,R$16)&amp;" by "&amp;IF(Q46&gt;R46,Q46-R46,R46-Q46)</f>
+      <c r="S46" s="42" t="str">
+        <f t="shared" si="16"/>
         <v>June by 3.50506100000001</v>
       </c>
-      <c r="T46" s="41">
-        <f t="shared" si="16"/>
+      <c r="T46" s="31">
+        <f t="shared" si="19"/>
         <v>8.0956486486487272E-3</v>
       </c>
-      <c r="U46" s="42">
-        <f t="shared" si="17"/>
+      <c r="U46" s="32">
+        <f t="shared" si="20"/>
         <v>-1.3212325609657817E-3</v>
       </c>
     </row>
@@ -2982,23 +3026,23 @@
         <v>2014</v>
       </c>
       <c r="Q47" s="6">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>75.027906999999999</v>
       </c>
       <c r="R47" s="12">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>69.896861000000001</v>
       </c>
-      <c r="S47" s="52" t="str">
-        <f>IF(Q47&gt;R47,Q$16,R$16)&amp;" by "&amp;IF(Q47&gt;R47,Q47-R47,R47-Q47)</f>
+      <c r="S47" s="42" t="str">
+        <f t="shared" si="16"/>
         <v>June by 5.131046</v>
       </c>
-      <c r="T47" s="41">
-        <f t="shared" si="16"/>
+      <c r="T47" s="31">
+        <f t="shared" si="19"/>
         <v>5.7484490626009237E-3</v>
       </c>
-      <c r="U47" s="42">
-        <f t="shared" si="17"/>
+      <c r="U47" s="32">
+        <f t="shared" si="20"/>
         <v>-1.6839054121811581E-2</v>
       </c>
     </row>
@@ -3031,23 +3075,23 @@
         <v>2015</v>
       </c>
       <c r="Q48" s="6">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>74.990148000000005</v>
       </c>
       <c r="R48" s="12">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>73.423912999999999</v>
       </c>
-      <c r="S48" s="52" t="str">
-        <f>IF(Q48&gt;R48,Q$16,R$16)&amp;" by "&amp;IF(Q48&gt;R48,Q48-R48,R48-Q48)</f>
+      <c r="S48" s="42" t="str">
+        <f t="shared" si="16"/>
         <v>June by 1.56623500000001</v>
       </c>
-      <c r="T48" s="41">
-        <f t="shared" si="16"/>
+      <c r="T48" s="31">
+        <f t="shared" si="19"/>
         <v>-5.0326607138320018E-4</v>
       </c>
-      <c r="U48" s="42">
-        <f t="shared" si="17"/>
+      <c r="U48" s="32">
+        <f t="shared" si="20"/>
         <v>5.0460806816489193E-2</v>
       </c>
     </row>
@@ -3080,23 +3124,23 @@
         <v>2016</v>
       </c>
       <c r="Q49" s="6">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>75.175257999999999</v>
       </c>
       <c r="R49" s="12">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>71.13</v>
       </c>
-      <c r="S49" s="52" t="str">
-        <f>IF(Q49&gt;R49,Q$16,R$16)&amp;" by "&amp;IF(Q49&gt;R49,Q49-R49,R49-Q49)</f>
+      <c r="S49" s="42" t="str">
+        <f t="shared" si="16"/>
         <v>June by 4.045258</v>
       </c>
-      <c r="T49" s="41">
-        <f t="shared" si="16"/>
+      <c r="T49" s="31">
+        <f t="shared" si="19"/>
         <v>2.4684575899222728E-3</v>
       </c>
-      <c r="U49" s="42">
-        <f t="shared" si="17"/>
+      <c r="U49" s="32">
+        <f t="shared" si="20"/>
         <v>-3.1242042357508288E-2</v>
       </c>
     </row>
@@ -3117,57 +3161,57 @@
         <v>41</v>
       </c>
       <c r="Q50" s="8">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>77.219894999999994</v>
       </c>
-      <c r="R50" s="48"/>
-      <c r="S50" s="54" t="str">
-        <f>IF(Q50&gt;R50,Q$16,R$16)&amp;" by "&amp;IF(Q50&gt;R50,Q50-R50,R50-Q50)</f>
+      <c r="R50" s="38"/>
+      <c r="S50" s="44" t="str">
+        <f t="shared" si="16"/>
         <v>June by 77.219895</v>
       </c>
-      <c r="T50" s="43">
-        <f t="shared" si="16"/>
+      <c r="T50" s="33">
+        <f t="shared" si="19"/>
         <v>2.7198270473511303E-2</v>
       </c>
-      <c r="U50" s="44">
-        <f t="shared" si="17"/>
+      <c r="U50" s="34">
+        <f t="shared" si="20"/>
         <v>-1</v>
       </c>
     </row>
     <row r="51" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="P51" s="37" t="s">
+      <c r="P51" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="Q51" s="55"/>
-      <c r="R51" s="55"/>
-      <c r="S51" s="45" t="s">
+      <c r="Q51" s="51"/>
+      <c r="R51" s="51"/>
+      <c r="S51" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="T51" s="46">
+      <c r="T51" s="36">
         <f>(Q49-Q43)/Q43</f>
         <v>3.3318109346309644E-3</v>
       </c>
-      <c r="U51" s="47">
+      <c r="U51" s="37">
         <f>(R49-R43)/R43</f>
         <v>1.3125032661638331E-2</v>
       </c>
     </row>
     <row r="52" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="P52" s="38"/>
-      <c r="Q52" s="38"/>
-      <c r="R52" s="38"/>
-      <c r="V52" s="34"/>
+      <c r="P52" s="52"/>
+      <c r="Q52" s="52"/>
+      <c r="R52" s="52"/>
+      <c r="V52" s="26"/>
     </row>
     <row r="53" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="P53" s="31" t="s">
+      <c r="P53" s="47" t="s">
         <v>51</v>
       </c>
-      <c r="Q53" s="32"/>
-      <c r="R53" s="32"/>
-      <c r="S53" s="33"/>
+      <c r="Q53" s="48"/>
+      <c r="R53" s="48"/>
+      <c r="S53" s="49"/>
       <c r="T53"/>
       <c r="U53"/>
-      <c r="V53" s="34"/>
+      <c r="V53" s="26"/>
     </row>
     <row r="54" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B54" s="16" t="s">
@@ -3176,12 +3220,12 @@
       <c r="I54" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="P54" s="25"/>
-      <c r="Q54" s="19" t="s">
+      <c r="P54" s="23"/>
+      <c r="Q54" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="R54" s="20"/>
-      <c r="S54" s="26"/>
+      <c r="R54" s="46"/>
+      <c r="S54" s="24"/>
       <c r="T54"/>
       <c r="U54"/>
     </row>
@@ -3231,7 +3275,7 @@
       <c r="R55" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="S55" s="24" t="s">
+      <c r="S55" s="22" t="s">
         <v>36</v>
       </c>
       <c r="T55"/>
@@ -3285,8 +3329,8 @@
         <f>K56</f>
         <v>151</v>
       </c>
-      <c r="S56" s="21" t="str">
-        <f>IF(Q56&gt;R56,Q$16,R$16)&amp;" by "&amp;IF(Q56&gt;R56,Q56-R56,R56-Q56)</f>
+      <c r="S56" s="19" t="str">
+        <f t="shared" ref="S56:S64" si="21">IF(Q56&gt;R56,Q$16,R$16)&amp;" by "&amp;IF(Q56&gt;R56,Q56-R56,R56-Q56)</f>
         <v>June by 8</v>
       </c>
       <c r="T56"/>
@@ -3333,15 +3377,15 @@
         <v>20</v>
       </c>
       <c r="Q57" s="6">
-        <f t="shared" ref="Q57:Q64" si="18">D57</f>
+        <f t="shared" ref="Q57:Q64" si="22">D57</f>
         <v>234</v>
       </c>
       <c r="R57" s="12">
-        <f t="shared" ref="R57:R64" si="19">K57</f>
+        <f t="shared" ref="R57:R64" si="23">K57</f>
         <v>216</v>
       </c>
-      <c r="S57" s="22" t="str">
-        <f>IF(Q57&gt;R57,Q$16,R$16)&amp;" by "&amp;IF(Q57&gt;R57,Q57-R57,R57-Q57)</f>
+      <c r="S57" s="20" t="str">
+        <f t="shared" si="21"/>
         <v>June by 18</v>
       </c>
       <c r="T57"/>
@@ -3388,15 +3432,15 @@
         <v>21</v>
       </c>
       <c r="Q58" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>167</v>
       </c>
       <c r="R58" s="12">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>147</v>
       </c>
-      <c r="S58" s="22" t="str">
-        <f>IF(Q58&gt;R58,Q$16,R$16)&amp;" by "&amp;IF(Q58&gt;R58,Q58-R58,R58-Q58)</f>
+      <c r="S58" s="20" t="str">
+        <f t="shared" si="21"/>
         <v>June by 20</v>
       </c>
       <c r="T58"/>
@@ -3443,15 +3487,15 @@
         <v>22</v>
       </c>
       <c r="Q59" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>214</v>
       </c>
       <c r="R59" s="12">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>197</v>
       </c>
-      <c r="S59" s="22" t="str">
-        <f>IF(Q59&gt;R59,Q$16,R$16)&amp;" by "&amp;IF(Q59&gt;R59,Q59-R59,R59-Q59)</f>
+      <c r="S59" s="20" t="str">
+        <f t="shared" si="21"/>
         <v>June by 17</v>
       </c>
       <c r="T59"/>
@@ -3498,15 +3542,15 @@
         <v>23</v>
       </c>
       <c r="Q60" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>79</v>
       </c>
       <c r="R60" s="12">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>55</v>
       </c>
-      <c r="S60" s="22" t="str">
-        <f>IF(Q60&gt;R60,Q$16,R$16)&amp;" by "&amp;IF(Q60&gt;R60,Q60-R60,R60-Q60)</f>
+      <c r="S60" s="20" t="str">
+        <f t="shared" si="21"/>
         <v>June by 24</v>
       </c>
       <c r="T60"/>
@@ -3553,15 +3597,15 @@
         <v>24</v>
       </c>
       <c r="Q61" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>26</v>
       </c>
       <c r="R61" s="12">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>11</v>
       </c>
-      <c r="S61" s="22" t="str">
-        <f>IF(Q61&gt;R61,Q$16,R$16)&amp;" by "&amp;IF(Q61&gt;R61,Q61-R61,R61-Q61)</f>
+      <c r="S61" s="20" t="str">
+        <f t="shared" si="21"/>
         <v>June by 15</v>
       </c>
       <c r="T61"/>
@@ -3608,15 +3652,15 @@
         <v>25</v>
       </c>
       <c r="Q62" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>236</v>
       </c>
       <c r="R62" s="12">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>217</v>
       </c>
-      <c r="S62" s="22" t="str">
-        <f>IF(Q62&gt;R62,Q$16,R$16)&amp;" by "&amp;IF(Q62&gt;R62,Q62-R62,R62-Q62)</f>
+      <c r="S62" s="20" t="str">
+        <f t="shared" si="21"/>
         <v>June by 19</v>
       </c>
       <c r="T62"/>
@@ -3663,15 +3707,15 @@
         <v>26</v>
       </c>
       <c r="Q63" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>233</v>
       </c>
       <c r="R63" s="12">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>207</v>
       </c>
-      <c r="S63" s="22" t="str">
-        <f>IF(Q63&gt;R63,Q$16,R$16)&amp;" by "&amp;IF(Q63&gt;R63,Q63-R63,R63-Q63)</f>
+      <c r="S63" s="20" t="str">
+        <f t="shared" si="21"/>
         <v>June by 26</v>
       </c>
       <c r="T63"/>
@@ -3718,34 +3762,34 @@
         <v>27</v>
       </c>
       <c r="Q64" s="8">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>226</v>
       </c>
       <c r="R64" s="14">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>204</v>
       </c>
-      <c r="S64" s="23" t="str">
-        <f>IF(Q64&gt;R64,Q$16,R$16)&amp;" by "&amp;IF(Q64&gt;R64,Q64-R64,R64-Q64)</f>
+      <c r="S64" s="21" t="str">
+        <f t="shared" si="21"/>
         <v>June by 22</v>
       </c>
       <c r="T64"/>
       <c r="U64"/>
     </row>
     <row r="65" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="P65" s="50"/>
-      <c r="Q65" s="53"/>
-      <c r="R65" s="53"/>
+      <c r="P65" s="40"/>
+      <c r="Q65" s="43"/>
+      <c r="R65" s="43"/>
       <c r="T65"/>
       <c r="U65"/>
     </row>
     <row r="66" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="P66" s="31" t="s">
+      <c r="P66" s="47" t="s">
         <v>51</v>
       </c>
-      <c r="Q66" s="32"/>
-      <c r="R66" s="32"/>
-      <c r="S66" s="33"/>
+      <c r="Q66" s="48"/>
+      <c r="R66" s="48"/>
+      <c r="S66" s="49"/>
     </row>
     <row r="67" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B67" s="16" t="s">
@@ -3754,12 +3798,12 @@
       <c r="I67" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="P67" s="25"/>
-      <c r="Q67" s="19" t="s">
+      <c r="P67" s="23"/>
+      <c r="Q67" s="45" t="s">
         <v>45</v>
       </c>
-      <c r="R67" s="20"/>
-      <c r="S67" s="26"/>
+      <c r="R67" s="46"/>
+      <c r="S67" s="24"/>
     </row>
     <row r="68" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B68" s="1" t="s">
@@ -3801,7 +3845,7 @@
       <c r="R68" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="S68" s="24" t="s">
+      <c r="S68" s="22" t="s">
         <v>36</v>
       </c>
     </row>
@@ -3847,8 +3891,8 @@
         <f>J69</f>
         <v>20.86</v>
       </c>
-      <c r="S69" s="21" t="str">
-        <f>IF(Q69&gt;R69,Q$16,R$16)&amp;" by "&amp;IF(Q69&gt;R69,Q69-R69,R69-Q69)</f>
+      <c r="S69" s="19" t="str">
+        <f t="shared" ref="S69:S77" si="24">IF(Q69&gt;R69,Q$16,R$16)&amp;" by "&amp;IF(Q69&gt;R69,Q69-R69,R69-Q69)</f>
         <v>December by 18.45</v>
       </c>
     </row>
@@ -3887,15 +3931,15 @@
         <v>20</v>
       </c>
       <c r="Q70" s="6">
-        <f t="shared" ref="Q70:Q77" si="20">C70</f>
+        <f t="shared" ref="Q70:Q77" si="25">C70</f>
         <v>27.67</v>
       </c>
       <c r="R70" s="12">
-        <f t="shared" ref="R70:R77" si="21">J70</f>
+        <f t="shared" ref="R70:R77" si="26">J70</f>
         <v>43.9</v>
       </c>
-      <c r="S70" s="22" t="str">
-        <f>IF(Q70&gt;R70,Q$16,R$16)&amp;" by "&amp;IF(Q70&gt;R70,Q70-R70,R70-Q70)</f>
+      <c r="S70" s="20" t="str">
+        <f t="shared" si="24"/>
         <v>December by 16.23</v>
       </c>
     </row>
@@ -3934,15 +3978,15 @@
         <v>21</v>
       </c>
       <c r="Q71" s="6">
-        <f t="shared" si="20"/>
+        <f t="shared" si="25"/>
         <v>19.07</v>
       </c>
       <c r="R71" s="12">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>22.78</v>
       </c>
-      <c r="S71" s="22" t="str">
-        <f>IF(Q71&gt;R71,Q$16,R$16)&amp;" by "&amp;IF(Q71&gt;R71,Q71-R71,R71-Q71)</f>
+      <c r="S71" s="20" t="str">
+        <f t="shared" si="24"/>
         <v>December by 3.71</v>
       </c>
     </row>
@@ -3981,15 +4025,15 @@
         <v>22</v>
       </c>
       <c r="Q72" s="6">
-        <f t="shared" si="20"/>
+        <f t="shared" si="25"/>
         <v>106.09</v>
       </c>
       <c r="R72" s="12">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>99.88</v>
       </c>
-      <c r="S72" s="22" t="str">
-        <f>IF(Q72&gt;R72,Q$16,R$16)&amp;" by "&amp;IF(Q72&gt;R72,Q72-R72,R72-Q72)</f>
+      <c r="S72" s="20" t="str">
+        <f t="shared" si="24"/>
         <v>June by 6.21000000000001</v>
       </c>
     </row>
@@ -4028,15 +4072,15 @@
         <v>23</v>
       </c>
       <c r="Q73" s="6">
-        <f t="shared" si="20"/>
+        <f t="shared" si="25"/>
         <v>4.58</v>
       </c>
       <c r="R73" s="12">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>8.4</v>
       </c>
-      <c r="S73" s="22" t="str">
-        <f>IF(Q73&gt;R73,Q$16,R$16)&amp;" by "&amp;IF(Q73&gt;R73,Q73-R73,R73-Q73)</f>
+      <c r="S73" s="20" t="str">
+        <f t="shared" si="24"/>
         <v>December by 3.82</v>
       </c>
     </row>
@@ -4075,15 +4119,15 @@
         <v>24</v>
       </c>
       <c r="Q74" s="6">
-        <f t="shared" si="20"/>
+        <f t="shared" si="25"/>
         <v>2.46</v>
       </c>
       <c r="R74" s="12">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>7.02</v>
       </c>
-      <c r="S74" s="22" t="str">
-        <f>IF(Q74&gt;R74,Q$16,R$16)&amp;" by "&amp;IF(Q74&gt;R74,Q74-R74,R74-Q74)</f>
+      <c r="S74" s="20" t="str">
+        <f t="shared" si="24"/>
         <v>December by 4.56</v>
       </c>
     </row>
@@ -4122,15 +4166,15 @@
         <v>25</v>
       </c>
       <c r="Q75" s="6">
-        <f t="shared" si="20"/>
+        <f t="shared" si="25"/>
         <v>35.76</v>
       </c>
       <c r="R75" s="12">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>53.15</v>
       </c>
-      <c r="S75" s="22" t="str">
-        <f>IF(Q75&gt;R75,Q$16,R$16)&amp;" by "&amp;IF(Q75&gt;R75,Q75-R75,R75-Q75)</f>
+      <c r="S75" s="20" t="str">
+        <f t="shared" si="24"/>
         <v>December by 17.39</v>
       </c>
     </row>
@@ -4169,15 +4213,15 @@
         <v>26</v>
       </c>
       <c r="Q76" s="6">
-        <f t="shared" si="20"/>
+        <f t="shared" si="25"/>
         <v>5.28</v>
       </c>
       <c r="R76" s="12">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>15.59</v>
       </c>
-      <c r="S76" s="22" t="str">
-        <f>IF(Q76&gt;R76,Q$16,R$16)&amp;" by "&amp;IF(Q76&gt;R76,Q76-R76,R76-Q76)</f>
+      <c r="S76" s="20" t="str">
+        <f t="shared" si="24"/>
         <v>December by 10.31</v>
       </c>
     </row>
@@ -4216,26 +4260,26 @@
         <v>27</v>
       </c>
       <c r="Q77" s="8">
-        <f t="shared" si="20"/>
+        <f t="shared" si="25"/>
         <v>11.31</v>
       </c>
       <c r="R77" s="14">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>33.049999999999997</v>
       </c>
-      <c r="S77" s="23" t="str">
-        <f>IF(Q77&gt;R77,Q$16,R$16)&amp;" by "&amp;IF(Q77&gt;R77,Q77-R77,R77-Q77)</f>
+      <c r="S77" s="21" t="str">
+        <f t="shared" si="24"/>
         <v>December by 21.74</v>
       </c>
     </row>
     <row r="78" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="79" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="P79" s="31" t="s">
+      <c r="P79" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="Q79" s="32"/>
-      <c r="R79" s="32"/>
-      <c r="S79" s="33"/>
+      <c r="Q79" s="48"/>
+      <c r="R79" s="48"/>
+      <c r="S79" s="49"/>
     </row>
     <row r="80" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B80" s="16" t="s">
@@ -4244,12 +4288,12 @@
       <c r="I80" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="P80" s="25"/>
-      <c r="Q80" s="19" t="s">
+      <c r="P80" s="23"/>
+      <c r="Q80" s="45" t="s">
         <v>48</v>
       </c>
-      <c r="R80" s="20"/>
-      <c r="S80" s="26"/>
+      <c r="R80" s="46"/>
+      <c r="S80" s="24"/>
     </row>
     <row r="81" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B81" s="1" t="s">
@@ -4291,7 +4335,7 @@
       <c r="R81" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="S81" s="24" t="s">
+      <c r="S81" s="22" t="s">
         <v>36</v>
       </c>
     </row>
@@ -4337,8 +4381,8 @@
         <f>K82</f>
         <v>69.684211000000005</v>
       </c>
-      <c r="S82" s="21" t="str">
-        <f>IF(Q82&gt;R82,Q$16,R$16)&amp;" by "&amp;IF(Q82&gt;R82,Q82-R82,R82-Q82)</f>
+      <c r="S82" s="19" t="str">
+        <f t="shared" ref="S82:S90" si="27">IF(Q82&gt;R82,Q$16,R$16)&amp;" by "&amp;IF(Q82&gt;R82,Q82-R82,R82-Q82)</f>
         <v>June by 4.45518299999999</v>
       </c>
     </row>
@@ -4377,15 +4421,15 @@
         <v>20</v>
       </c>
       <c r="Q83" s="6">
-        <f t="shared" ref="Q83:Q90" si="22">D83</f>
+        <f t="shared" ref="Q83:Q90" si="28">D83</f>
         <v>74.050847000000005</v>
       </c>
       <c r="R83" s="12">
-        <f t="shared" ref="R83:R90" si="23">K83</f>
+        <f t="shared" ref="R83:R90" si="29">K83</f>
         <v>71.069444000000004</v>
       </c>
-      <c r="S83" s="22" t="str">
-        <f>IF(Q83&gt;R83,Q$16,R$16)&amp;" by "&amp;IF(Q83&gt;R83,Q83-R83,R83-Q83)</f>
+      <c r="S83" s="20" t="str">
+        <f t="shared" si="27"/>
         <v>June by 2.981403</v>
       </c>
     </row>
@@ -4424,15 +4468,15 @@
         <v>21</v>
       </c>
       <c r="Q84" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="28"/>
         <v>76.005375999999998</v>
       </c>
       <c r="R84" s="12">
-        <f t="shared" si="23"/>
+        <f t="shared" si="29"/>
         <v>73.224718999999993</v>
       </c>
-      <c r="S84" s="22" t="str">
-        <f>IF(Q84&gt;R84,Q$16,R$16)&amp;" by "&amp;IF(Q84&gt;R84,Q84-R84,R84-Q84)</f>
+      <c r="S84" s="20" t="str">
+        <f t="shared" si="27"/>
         <v>June by 2.78065700000001</v>
       </c>
     </row>
@@ -4471,15 +4515,15 @@
         <v>22</v>
       </c>
       <c r="Q85" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="28"/>
         <v>71.937219999999996</v>
       </c>
       <c r="R85" s="12">
-        <f t="shared" si="23"/>
+        <f t="shared" si="29"/>
         <v>69.291262000000003</v>
       </c>
-      <c r="S85" s="22" t="str">
-        <f>IF(Q85&gt;R85,Q$16,R$16)&amp;" by "&amp;IF(Q85&gt;R85,Q85-R85,R85-Q85)</f>
+      <c r="S85" s="20" t="str">
+        <f t="shared" si="27"/>
         <v>June by 2.64595799999999</v>
       </c>
     </row>
@@ -4518,15 +4562,15 @@
         <v>23</v>
       </c>
       <c r="Q86" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="28"/>
         <v>76.655405000000002</v>
       </c>
       <c r="R86" s="12">
-        <f t="shared" si="23"/>
+        <f t="shared" si="29"/>
         <v>71.834862000000001</v>
       </c>
-      <c r="S86" s="22" t="str">
-        <f>IF(Q86&gt;R86,Q$16,R$16)&amp;" by "&amp;IF(Q86&gt;R86,Q86-R86,R86-Q86)</f>
+      <c r="S86" s="20" t="str">
+        <f t="shared" si="27"/>
         <v>June by 4.820543</v>
       </c>
     </row>
@@ -4565,15 +4609,15 @@
         <v>24</v>
       </c>
       <c r="Q87" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="28"/>
         <v>73.394737000000006</v>
       </c>
       <c r="R87" s="12">
-        <f t="shared" si="23"/>
+        <f t="shared" si="29"/>
         <v>72.421053000000001</v>
       </c>
-      <c r="S87" s="22" t="str">
-        <f>IF(Q87&gt;R87,Q$16,R$16)&amp;" by "&amp;IF(Q87&gt;R87,Q87-R87,R87-Q87)</f>
+      <c r="S87" s="20" t="str">
+        <f t="shared" si="27"/>
         <v>June by 0.973684000000006</v>
       </c>
     </row>
@@ -4612,15 +4656,15 @@
         <v>25</v>
       </c>
       <c r="Q88" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="28"/>
         <v>73.271186</v>
       </c>
       <c r="R88" s="12">
-        <f t="shared" si="23"/>
+        <f t="shared" si="29"/>
         <v>69.903226000000004</v>
       </c>
-      <c r="S88" s="22" t="str">
-        <f>IF(Q88&gt;R88,Q$16,R$16)&amp;" by "&amp;IF(Q88&gt;R88,Q88-R88,R88-Q88)</f>
+      <c r="S88" s="20" t="str">
+        <f t="shared" si="27"/>
         <v>June by 3.36796</v>
       </c>
     </row>
@@ -4659,15 +4703,15 @@
         <v>26</v>
       </c>
       <c r="Q89" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="28"/>
         <v>77.559321999999995</v>
       </c>
       <c r="R89" s="12">
-        <f t="shared" si="23"/>
+        <f t="shared" si="29"/>
         <v>71.109523999999993</v>
       </c>
-      <c r="S89" s="22" t="str">
-        <f>IF(Q89&gt;R89,Q$16,R$16)&amp;" by "&amp;IF(Q89&gt;R89,Q89-R89,R89-Q89)</f>
+      <c r="S89" s="20" t="str">
+        <f t="shared" si="27"/>
         <v>June by 6.449798</v>
       </c>
     </row>
@@ -4706,20 +4750,25 @@
         <v>27</v>
       </c>
       <c r="Q90" s="8">
-        <f t="shared" si="22"/>
+        <f t="shared" si="28"/>
         <v>76.668103000000002</v>
       </c>
       <c r="R90" s="14">
-        <f t="shared" si="23"/>
+        <f t="shared" si="29"/>
         <v>72.433333000000005</v>
       </c>
-      <c r="S90" s="23" t="str">
-        <f>IF(Q90&gt;R90,Q$16,R$16)&amp;" by "&amp;IF(Q90&gt;R90,Q90-R90,R90-Q90)</f>
+      <c r="S90" s="21" t="str">
+        <f t="shared" si="27"/>
         <v>June by 4.23477</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="T3:U3"/>
+    <mergeCell ref="P2:V2"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="T15:U15"/>
     <mergeCell ref="Q67:R67"/>
     <mergeCell ref="P79:S79"/>
     <mergeCell ref="Q80:R80"/>
@@ -4736,37 +4785,24 @@
     <mergeCell ref="Q28:R28"/>
     <mergeCell ref="T28:U28"/>
     <mergeCell ref="P38:R39"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="T3:U3"/>
-    <mergeCell ref="P2:V2"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="T15:U15"/>
   </mergeCells>
   <conditionalFormatting sqref="T18:U24 T31:U37">
-    <cfRule type="cellIs" dxfId="5" priority="43" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="43" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="44" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="44" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T44:U50">
-    <cfRule type="cellIs" dxfId="3" priority="41" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="41" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="42" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="42" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q56:Q64">
-    <cfRule type="colorScale" priority="38">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF92D050"/>
-        <color rgb="FFFF0000"/>
-      </colorScale>
-    </cfRule>
     <cfRule type="colorScale" priority="37">
       <colorScale>
         <cfvo type="min"/>
@@ -4775,6 +4811,14 @@
         <color theme="0"/>
         <color rgb="FFFFC000"/>
         <color rgb="FF00B0F0"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="38">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF92D050"/>
+        <color rgb="FFFF0000"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
@@ -5058,6 +5102,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>